<commit_message>
app field analysis for unknown parasource
</commit_message>
<xml_diff>
--- a/results analysis.xlsx
+++ b/results analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="19416" windowHeight="10416" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="All-v10" sheetId="8" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13011" uniqueCount="1197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13012" uniqueCount="1199">
   <si>
     <t>A</t>
   </si>
@@ -3683,10 +3683,6 @@
     <t>cgeo.geocaching-23234767</t>
   </si>
   <si>
-    <t>&lt;android.content.ContextWrapper: android.content.Intent registerReceiver(android.content.BroadcastReceiver,android.content.IntentFilter)&gt; -&gt; &lt;android.app.ContextImpl: android.content.Intent registerReceiver(android.content.BroadcastReceiver,android.content.IntentFilter)&gt;</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>ParaAndField</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3696,6 +3692,18 @@
   </si>
   <si>
     <t>motivating example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>android.database.sqlite.SQLiteProgram.bindString</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>&lt;android.content.ContextWrapper: android.content.Intent registerReceiver(android.content.BroadcastReceiver,android.content.IntentFilter)&gt; -&gt;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> &lt;android.app.ContextImpl: android.content.Intent registerReceiver(android.content.BroadcastReceiver,android.content.IntentFilter)&gt;</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -5870,8 +5878,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z508"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A381" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A399" sqref="A399:XFD399"/>
+    <sheetView topLeftCell="A462" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C495" sqref="C495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -73375,10 +73383,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H72"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="C46" workbookViewId="0">
+      <selection activeCell="I62" sqref="I62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -73388,8 +73396,8 @@
     <col min="4" max="4" width="30.21875" customWidth="1"/>
     <col min="6" max="6" width="4.77734375" customWidth="1"/>
     <col min="7" max="7" width="4.44140625" customWidth="1"/>
-    <col min="8" max="8" width="99.33203125" customWidth="1"/>
-    <col min="9" max="9" width="101" customWidth="1"/>
+    <col min="8" max="8" width="58.109375" customWidth="1"/>
+    <col min="9" max="9" width="44.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -74511,7 +74519,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -74534,7 +74542,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -74557,7 +74565,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -74580,7 +74588,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -74603,7 +74611,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -74626,7 +74634,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -74649,7 +74657,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -74672,7 +74680,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -74695,7 +74703,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -74703,7 +74711,7 @@
         <v>1138</v>
       </c>
       <c r="C57" t="s">
-        <v>1139</v>
+        <v>1196</v>
       </c>
       <c r="D57" t="s">
         <v>1069</v>
@@ -74718,7 +74726,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -74741,7 +74749,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>1065</v>
       </c>
@@ -74764,7 +74772,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>5</v>
       </c>
@@ -74787,7 +74795,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="62" spans="1:8" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>5</v>
       </c>
@@ -74795,10 +74803,10 @@
         <v>1118</v>
       </c>
       <c r="C62" t="s">
-        <v>1195</v>
+        <v>1194</v>
       </c>
       <c r="D62" t="s">
-        <v>1194</v>
+        <v>1193</v>
       </c>
       <c r="E62">
         <v>3</v>
@@ -74810,10 +74818,13 @@
         <v>6</v>
       </c>
       <c r="H62" s="17" t="s">
-        <v>1193</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1197</v>
+      </c>
+      <c r="I62" s="17" t="s">
+        <v>1198</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>5</v>
       </c>
@@ -74836,7 +74847,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>5</v>
       </c>
@@ -74882,7 +74893,7 @@
         <v>3</v>
       </c>
       <c r="H65" t="s">
-        <v>1196</v>
+        <v>1195</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>